<commit_message>
[BI-1613] Update TAF to include term type
</commit_message>
<xml_diff>
--- a/src/files/TraitImport/test_import-xlsx.xlsx
+++ b/src/files/TraitImport/test_import-xlsx.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daw279\Documents\Testing\Cucumber\BI_Cucumber\TraitImportFiles\v0.5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/taf/src/files/TraitImport/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC8DA90-76C0-5647-8225-6C218DE403E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25428" windowHeight="12660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25420" windowHeight="12660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
   <si>
     <t>Column</t>
   </si>
@@ -278,12 +279,24 @@
   </si>
   <si>
     <t>Count unbroken square pretzels</t>
+  </si>
+  <si>
+    <t>Term Type</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>Germplasm ATTRIBUTE</t>
+  </si>
+  <si>
+    <t>germplasm passport</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -394,16 +407,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -413,7 +422,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -429,12 +437,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,468 +876,404 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19" style="22" customWidth="1"/>
-    <col min="2" max="2" width="79" style="22" customWidth="1"/>
-    <col min="3" max="3" width="76.6640625" style="23" customWidth="1"/>
-    <col min="4" max="256" width="11.5" style="4"/>
-    <col min="257" max="257" width="19" style="4" customWidth="1"/>
-    <col min="258" max="258" width="79" style="4" customWidth="1"/>
-    <col min="259" max="259" width="76.6640625" style="4" customWidth="1"/>
-    <col min="260" max="512" width="11.5" style="4"/>
-    <col min="513" max="513" width="19" style="4" customWidth="1"/>
-    <col min="514" max="514" width="79" style="4" customWidth="1"/>
-    <col min="515" max="515" width="76.6640625" style="4" customWidth="1"/>
-    <col min="516" max="768" width="11.5" style="4"/>
-    <col min="769" max="769" width="19" style="4" customWidth="1"/>
-    <col min="770" max="770" width="79" style="4" customWidth="1"/>
-    <col min="771" max="771" width="76.6640625" style="4" customWidth="1"/>
-    <col min="772" max="1024" width="11.5" style="4"/>
-    <col min="1025" max="1025" width="19" style="4" customWidth="1"/>
-    <col min="1026" max="1026" width="79" style="4" customWidth="1"/>
-    <col min="1027" max="1027" width="76.6640625" style="4" customWidth="1"/>
-    <col min="1028" max="1280" width="11.5" style="4"/>
-    <col min="1281" max="1281" width="19" style="4" customWidth="1"/>
-    <col min="1282" max="1282" width="79" style="4" customWidth="1"/>
-    <col min="1283" max="1283" width="76.6640625" style="4" customWidth="1"/>
-    <col min="1284" max="1536" width="11.5" style="4"/>
-    <col min="1537" max="1537" width="19" style="4" customWidth="1"/>
-    <col min="1538" max="1538" width="79" style="4" customWidth="1"/>
-    <col min="1539" max="1539" width="76.6640625" style="4" customWidth="1"/>
-    <col min="1540" max="1792" width="11.5" style="4"/>
-    <col min="1793" max="1793" width="19" style="4" customWidth="1"/>
-    <col min="1794" max="1794" width="79" style="4" customWidth="1"/>
-    <col min="1795" max="1795" width="76.6640625" style="4" customWidth="1"/>
-    <col min="1796" max="2048" width="11.5" style="4"/>
-    <col min="2049" max="2049" width="19" style="4" customWidth="1"/>
-    <col min="2050" max="2050" width="79" style="4" customWidth="1"/>
-    <col min="2051" max="2051" width="76.6640625" style="4" customWidth="1"/>
-    <col min="2052" max="2304" width="11.5" style="4"/>
-    <col min="2305" max="2305" width="19" style="4" customWidth="1"/>
-    <col min="2306" max="2306" width="79" style="4" customWidth="1"/>
-    <col min="2307" max="2307" width="76.6640625" style="4" customWidth="1"/>
-    <col min="2308" max="2560" width="11.5" style="4"/>
-    <col min="2561" max="2561" width="19" style="4" customWidth="1"/>
-    <col min="2562" max="2562" width="79" style="4" customWidth="1"/>
-    <col min="2563" max="2563" width="76.6640625" style="4" customWidth="1"/>
-    <col min="2564" max="2816" width="11.5" style="4"/>
-    <col min="2817" max="2817" width="19" style="4" customWidth="1"/>
-    <col min="2818" max="2818" width="79" style="4" customWidth="1"/>
-    <col min="2819" max="2819" width="76.6640625" style="4" customWidth="1"/>
-    <col min="2820" max="3072" width="11.5" style="4"/>
-    <col min="3073" max="3073" width="19" style="4" customWidth="1"/>
-    <col min="3074" max="3074" width="79" style="4" customWidth="1"/>
-    <col min="3075" max="3075" width="76.6640625" style="4" customWidth="1"/>
-    <col min="3076" max="3328" width="11.5" style="4"/>
-    <col min="3329" max="3329" width="19" style="4" customWidth="1"/>
-    <col min="3330" max="3330" width="79" style="4" customWidth="1"/>
-    <col min="3331" max="3331" width="76.6640625" style="4" customWidth="1"/>
-    <col min="3332" max="3584" width="11.5" style="4"/>
-    <col min="3585" max="3585" width="19" style="4" customWidth="1"/>
-    <col min="3586" max="3586" width="79" style="4" customWidth="1"/>
-    <col min="3587" max="3587" width="76.6640625" style="4" customWidth="1"/>
-    <col min="3588" max="3840" width="11.5" style="4"/>
-    <col min="3841" max="3841" width="19" style="4" customWidth="1"/>
-    <col min="3842" max="3842" width="79" style="4" customWidth="1"/>
-    <col min="3843" max="3843" width="76.6640625" style="4" customWidth="1"/>
-    <col min="3844" max="4096" width="11.5" style="4"/>
-    <col min="4097" max="4097" width="19" style="4" customWidth="1"/>
-    <col min="4098" max="4098" width="79" style="4" customWidth="1"/>
-    <col min="4099" max="4099" width="76.6640625" style="4" customWidth="1"/>
-    <col min="4100" max="4352" width="11.5" style="4"/>
-    <col min="4353" max="4353" width="19" style="4" customWidth="1"/>
-    <col min="4354" max="4354" width="79" style="4" customWidth="1"/>
-    <col min="4355" max="4355" width="76.6640625" style="4" customWidth="1"/>
-    <col min="4356" max="4608" width="11.5" style="4"/>
-    <col min="4609" max="4609" width="19" style="4" customWidth="1"/>
-    <col min="4610" max="4610" width="79" style="4" customWidth="1"/>
-    <col min="4611" max="4611" width="76.6640625" style="4" customWidth="1"/>
-    <col min="4612" max="4864" width="11.5" style="4"/>
-    <col min="4865" max="4865" width="19" style="4" customWidth="1"/>
-    <col min="4866" max="4866" width="79" style="4" customWidth="1"/>
-    <col min="4867" max="4867" width="76.6640625" style="4" customWidth="1"/>
-    <col min="4868" max="5120" width="11.5" style="4"/>
-    <col min="5121" max="5121" width="19" style="4" customWidth="1"/>
-    <col min="5122" max="5122" width="79" style="4" customWidth="1"/>
-    <col min="5123" max="5123" width="76.6640625" style="4" customWidth="1"/>
-    <col min="5124" max="5376" width="11.5" style="4"/>
-    <col min="5377" max="5377" width="19" style="4" customWidth="1"/>
-    <col min="5378" max="5378" width="79" style="4" customWidth="1"/>
-    <col min="5379" max="5379" width="76.6640625" style="4" customWidth="1"/>
-    <col min="5380" max="5632" width="11.5" style="4"/>
-    <col min="5633" max="5633" width="19" style="4" customWidth="1"/>
-    <col min="5634" max="5634" width="79" style="4" customWidth="1"/>
-    <col min="5635" max="5635" width="76.6640625" style="4" customWidth="1"/>
-    <col min="5636" max="5888" width="11.5" style="4"/>
-    <col min="5889" max="5889" width="19" style="4" customWidth="1"/>
-    <col min="5890" max="5890" width="79" style="4" customWidth="1"/>
-    <col min="5891" max="5891" width="76.6640625" style="4" customWidth="1"/>
-    <col min="5892" max="6144" width="11.5" style="4"/>
-    <col min="6145" max="6145" width="19" style="4" customWidth="1"/>
-    <col min="6146" max="6146" width="79" style="4" customWidth="1"/>
-    <col min="6147" max="6147" width="76.6640625" style="4" customWidth="1"/>
-    <col min="6148" max="6400" width="11.5" style="4"/>
-    <col min="6401" max="6401" width="19" style="4" customWidth="1"/>
-    <col min="6402" max="6402" width="79" style="4" customWidth="1"/>
-    <col min="6403" max="6403" width="76.6640625" style="4" customWidth="1"/>
-    <col min="6404" max="6656" width="11.5" style="4"/>
-    <col min="6657" max="6657" width="19" style="4" customWidth="1"/>
-    <col min="6658" max="6658" width="79" style="4" customWidth="1"/>
-    <col min="6659" max="6659" width="76.6640625" style="4" customWidth="1"/>
-    <col min="6660" max="6912" width="11.5" style="4"/>
-    <col min="6913" max="6913" width="19" style="4" customWidth="1"/>
-    <col min="6914" max="6914" width="79" style="4" customWidth="1"/>
-    <col min="6915" max="6915" width="76.6640625" style="4" customWidth="1"/>
-    <col min="6916" max="7168" width="11.5" style="4"/>
-    <col min="7169" max="7169" width="19" style="4" customWidth="1"/>
-    <col min="7170" max="7170" width="79" style="4" customWidth="1"/>
-    <col min="7171" max="7171" width="76.6640625" style="4" customWidth="1"/>
-    <col min="7172" max="7424" width="11.5" style="4"/>
-    <col min="7425" max="7425" width="19" style="4" customWidth="1"/>
-    <col min="7426" max="7426" width="79" style="4" customWidth="1"/>
-    <col min="7427" max="7427" width="76.6640625" style="4" customWidth="1"/>
-    <col min="7428" max="7680" width="11.5" style="4"/>
-    <col min="7681" max="7681" width="19" style="4" customWidth="1"/>
-    <col min="7682" max="7682" width="79" style="4" customWidth="1"/>
-    <col min="7683" max="7683" width="76.6640625" style="4" customWidth="1"/>
-    <col min="7684" max="7936" width="11.5" style="4"/>
-    <col min="7937" max="7937" width="19" style="4" customWidth="1"/>
-    <col min="7938" max="7938" width="79" style="4" customWidth="1"/>
-    <col min="7939" max="7939" width="76.6640625" style="4" customWidth="1"/>
-    <col min="7940" max="8192" width="11.5" style="4"/>
-    <col min="8193" max="8193" width="19" style="4" customWidth="1"/>
-    <col min="8194" max="8194" width="79" style="4" customWidth="1"/>
-    <col min="8195" max="8195" width="76.6640625" style="4" customWidth="1"/>
-    <col min="8196" max="8448" width="11.5" style="4"/>
-    <col min="8449" max="8449" width="19" style="4" customWidth="1"/>
-    <col min="8450" max="8450" width="79" style="4" customWidth="1"/>
-    <col min="8451" max="8451" width="76.6640625" style="4" customWidth="1"/>
-    <col min="8452" max="8704" width="11.5" style="4"/>
-    <col min="8705" max="8705" width="19" style="4" customWidth="1"/>
-    <col min="8706" max="8706" width="79" style="4" customWidth="1"/>
-    <col min="8707" max="8707" width="76.6640625" style="4" customWidth="1"/>
-    <col min="8708" max="8960" width="11.5" style="4"/>
-    <col min="8961" max="8961" width="19" style="4" customWidth="1"/>
-    <col min="8962" max="8962" width="79" style="4" customWidth="1"/>
-    <col min="8963" max="8963" width="76.6640625" style="4" customWidth="1"/>
-    <col min="8964" max="9216" width="11.5" style="4"/>
-    <col min="9217" max="9217" width="19" style="4" customWidth="1"/>
-    <col min="9218" max="9218" width="79" style="4" customWidth="1"/>
-    <col min="9219" max="9219" width="76.6640625" style="4" customWidth="1"/>
-    <col min="9220" max="9472" width="11.5" style="4"/>
-    <col min="9473" max="9473" width="19" style="4" customWidth="1"/>
-    <col min="9474" max="9474" width="79" style="4" customWidth="1"/>
-    <col min="9475" max="9475" width="76.6640625" style="4" customWidth="1"/>
-    <col min="9476" max="9728" width="11.5" style="4"/>
-    <col min="9729" max="9729" width="19" style="4" customWidth="1"/>
-    <col min="9730" max="9730" width="79" style="4" customWidth="1"/>
-    <col min="9731" max="9731" width="76.6640625" style="4" customWidth="1"/>
-    <col min="9732" max="9984" width="11.5" style="4"/>
-    <col min="9985" max="9985" width="19" style="4" customWidth="1"/>
-    <col min="9986" max="9986" width="79" style="4" customWidth="1"/>
-    <col min="9987" max="9987" width="76.6640625" style="4" customWidth="1"/>
-    <col min="9988" max="10240" width="11.5" style="4"/>
-    <col min="10241" max="10241" width="19" style="4" customWidth="1"/>
-    <col min="10242" max="10242" width="79" style="4" customWidth="1"/>
-    <col min="10243" max="10243" width="76.6640625" style="4" customWidth="1"/>
-    <col min="10244" max="10496" width="11.5" style="4"/>
-    <col min="10497" max="10497" width="19" style="4" customWidth="1"/>
-    <col min="10498" max="10498" width="79" style="4" customWidth="1"/>
-    <col min="10499" max="10499" width="76.6640625" style="4" customWidth="1"/>
-    <col min="10500" max="10752" width="11.5" style="4"/>
-    <col min="10753" max="10753" width="19" style="4" customWidth="1"/>
-    <col min="10754" max="10754" width="79" style="4" customWidth="1"/>
-    <col min="10755" max="10755" width="76.6640625" style="4" customWidth="1"/>
-    <col min="10756" max="11008" width="11.5" style="4"/>
-    <col min="11009" max="11009" width="19" style="4" customWidth="1"/>
-    <col min="11010" max="11010" width="79" style="4" customWidth="1"/>
-    <col min="11011" max="11011" width="76.6640625" style="4" customWidth="1"/>
-    <col min="11012" max="11264" width="11.5" style="4"/>
-    <col min="11265" max="11265" width="19" style="4" customWidth="1"/>
-    <col min="11266" max="11266" width="79" style="4" customWidth="1"/>
-    <col min="11267" max="11267" width="76.6640625" style="4" customWidth="1"/>
-    <col min="11268" max="11520" width="11.5" style="4"/>
-    <col min="11521" max="11521" width="19" style="4" customWidth="1"/>
-    <col min="11522" max="11522" width="79" style="4" customWidth="1"/>
-    <col min="11523" max="11523" width="76.6640625" style="4" customWidth="1"/>
-    <col min="11524" max="11776" width="11.5" style="4"/>
-    <col min="11777" max="11777" width="19" style="4" customWidth="1"/>
-    <col min="11778" max="11778" width="79" style="4" customWidth="1"/>
-    <col min="11779" max="11779" width="76.6640625" style="4" customWidth="1"/>
-    <col min="11780" max="12032" width="11.5" style="4"/>
-    <col min="12033" max="12033" width="19" style="4" customWidth="1"/>
-    <col min="12034" max="12034" width="79" style="4" customWidth="1"/>
-    <col min="12035" max="12035" width="76.6640625" style="4" customWidth="1"/>
-    <col min="12036" max="12288" width="11.5" style="4"/>
-    <col min="12289" max="12289" width="19" style="4" customWidth="1"/>
-    <col min="12290" max="12290" width="79" style="4" customWidth="1"/>
-    <col min="12291" max="12291" width="76.6640625" style="4" customWidth="1"/>
-    <col min="12292" max="12544" width="11.5" style="4"/>
-    <col min="12545" max="12545" width="19" style="4" customWidth="1"/>
-    <col min="12546" max="12546" width="79" style="4" customWidth="1"/>
-    <col min="12547" max="12547" width="76.6640625" style="4" customWidth="1"/>
-    <col min="12548" max="12800" width="11.5" style="4"/>
-    <col min="12801" max="12801" width="19" style="4" customWidth="1"/>
-    <col min="12802" max="12802" width="79" style="4" customWidth="1"/>
-    <col min="12803" max="12803" width="76.6640625" style="4" customWidth="1"/>
-    <col min="12804" max="13056" width="11.5" style="4"/>
-    <col min="13057" max="13057" width="19" style="4" customWidth="1"/>
-    <col min="13058" max="13058" width="79" style="4" customWidth="1"/>
-    <col min="13059" max="13059" width="76.6640625" style="4" customWidth="1"/>
-    <col min="13060" max="13312" width="11.5" style="4"/>
-    <col min="13313" max="13313" width="19" style="4" customWidth="1"/>
-    <col min="13314" max="13314" width="79" style="4" customWidth="1"/>
-    <col min="13315" max="13315" width="76.6640625" style="4" customWidth="1"/>
-    <col min="13316" max="13568" width="11.5" style="4"/>
-    <col min="13569" max="13569" width="19" style="4" customWidth="1"/>
-    <col min="13570" max="13570" width="79" style="4" customWidth="1"/>
-    <col min="13571" max="13571" width="76.6640625" style="4" customWidth="1"/>
-    <col min="13572" max="13824" width="11.5" style="4"/>
-    <col min="13825" max="13825" width="19" style="4" customWidth="1"/>
-    <col min="13826" max="13826" width="79" style="4" customWidth="1"/>
-    <col min="13827" max="13827" width="76.6640625" style="4" customWidth="1"/>
-    <col min="13828" max="14080" width="11.5" style="4"/>
-    <col min="14081" max="14081" width="19" style="4" customWidth="1"/>
-    <col min="14082" max="14082" width="79" style="4" customWidth="1"/>
-    <col min="14083" max="14083" width="76.6640625" style="4" customWidth="1"/>
-    <col min="14084" max="14336" width="11.5" style="4"/>
-    <col min="14337" max="14337" width="19" style="4" customWidth="1"/>
-    <col min="14338" max="14338" width="79" style="4" customWidth="1"/>
-    <col min="14339" max="14339" width="76.6640625" style="4" customWidth="1"/>
-    <col min="14340" max="14592" width="11.5" style="4"/>
-    <col min="14593" max="14593" width="19" style="4" customWidth="1"/>
-    <col min="14594" max="14594" width="79" style="4" customWidth="1"/>
-    <col min="14595" max="14595" width="76.6640625" style="4" customWidth="1"/>
-    <col min="14596" max="14848" width="11.5" style="4"/>
-    <col min="14849" max="14849" width="19" style="4" customWidth="1"/>
-    <col min="14850" max="14850" width="79" style="4" customWidth="1"/>
-    <col min="14851" max="14851" width="76.6640625" style="4" customWidth="1"/>
-    <col min="14852" max="15104" width="11.5" style="4"/>
-    <col min="15105" max="15105" width="19" style="4" customWidth="1"/>
-    <col min="15106" max="15106" width="79" style="4" customWidth="1"/>
-    <col min="15107" max="15107" width="76.6640625" style="4" customWidth="1"/>
-    <col min="15108" max="15360" width="11.5" style="4"/>
-    <col min="15361" max="15361" width="19" style="4" customWidth="1"/>
-    <col min="15362" max="15362" width="79" style="4" customWidth="1"/>
-    <col min="15363" max="15363" width="76.6640625" style="4" customWidth="1"/>
-    <col min="15364" max="15616" width="11.5" style="4"/>
-    <col min="15617" max="15617" width="19" style="4" customWidth="1"/>
-    <col min="15618" max="15618" width="79" style="4" customWidth="1"/>
-    <col min="15619" max="15619" width="76.6640625" style="4" customWidth="1"/>
-    <col min="15620" max="15872" width="11.5" style="4"/>
-    <col min="15873" max="15873" width="19" style="4" customWidth="1"/>
-    <col min="15874" max="15874" width="79" style="4" customWidth="1"/>
-    <col min="15875" max="15875" width="76.6640625" style="4" customWidth="1"/>
-    <col min="15876" max="16128" width="11.5" style="4"/>
-    <col min="16129" max="16129" width="19" style="4" customWidth="1"/>
-    <col min="16130" max="16130" width="79" style="4" customWidth="1"/>
-    <col min="16131" max="16131" width="76.6640625" style="4" customWidth="1"/>
-    <col min="16132" max="16384" width="11.5" style="4"/>
+    <col min="1" max="1" width="19" style="19" customWidth="1"/>
+    <col min="2" max="2" width="79" style="19" customWidth="1"/>
+    <col min="3" max="3" width="76.6640625" style="19" customWidth="1"/>
+    <col min="257" max="257" width="19" customWidth="1"/>
+    <col min="258" max="258" width="79" customWidth="1"/>
+    <col min="259" max="259" width="76.6640625" customWidth="1"/>
+    <col min="513" max="513" width="19" customWidth="1"/>
+    <col min="514" max="514" width="79" customWidth="1"/>
+    <col min="515" max="515" width="76.6640625" customWidth="1"/>
+    <col min="769" max="769" width="19" customWidth="1"/>
+    <col min="770" max="770" width="79" customWidth="1"/>
+    <col min="771" max="771" width="76.6640625" customWidth="1"/>
+    <col min="1025" max="1025" width="19" customWidth="1"/>
+    <col min="1026" max="1026" width="79" customWidth="1"/>
+    <col min="1027" max="1027" width="76.6640625" customWidth="1"/>
+    <col min="1281" max="1281" width="19" customWidth="1"/>
+    <col min="1282" max="1282" width="79" customWidth="1"/>
+    <col min="1283" max="1283" width="76.6640625" customWidth="1"/>
+    <col min="1537" max="1537" width="19" customWidth="1"/>
+    <col min="1538" max="1538" width="79" customWidth="1"/>
+    <col min="1539" max="1539" width="76.6640625" customWidth="1"/>
+    <col min="1793" max="1793" width="19" customWidth="1"/>
+    <col min="1794" max="1794" width="79" customWidth="1"/>
+    <col min="1795" max="1795" width="76.6640625" customWidth="1"/>
+    <col min="2049" max="2049" width="19" customWidth="1"/>
+    <col min="2050" max="2050" width="79" customWidth="1"/>
+    <col min="2051" max="2051" width="76.6640625" customWidth="1"/>
+    <col min="2305" max="2305" width="19" customWidth="1"/>
+    <col min="2306" max="2306" width="79" customWidth="1"/>
+    <col min="2307" max="2307" width="76.6640625" customWidth="1"/>
+    <col min="2561" max="2561" width="19" customWidth="1"/>
+    <col min="2562" max="2562" width="79" customWidth="1"/>
+    <col min="2563" max="2563" width="76.6640625" customWidth="1"/>
+    <col min="2817" max="2817" width="19" customWidth="1"/>
+    <col min="2818" max="2818" width="79" customWidth="1"/>
+    <col min="2819" max="2819" width="76.6640625" customWidth="1"/>
+    <col min="3073" max="3073" width="19" customWidth="1"/>
+    <col min="3074" max="3074" width="79" customWidth="1"/>
+    <col min="3075" max="3075" width="76.6640625" customWidth="1"/>
+    <col min="3329" max="3329" width="19" customWidth="1"/>
+    <col min="3330" max="3330" width="79" customWidth="1"/>
+    <col min="3331" max="3331" width="76.6640625" customWidth="1"/>
+    <col min="3585" max="3585" width="19" customWidth="1"/>
+    <col min="3586" max="3586" width="79" customWidth="1"/>
+    <col min="3587" max="3587" width="76.6640625" customWidth="1"/>
+    <col min="3841" max="3841" width="19" customWidth="1"/>
+    <col min="3842" max="3842" width="79" customWidth="1"/>
+    <col min="3843" max="3843" width="76.6640625" customWidth="1"/>
+    <col min="4097" max="4097" width="19" customWidth="1"/>
+    <col min="4098" max="4098" width="79" customWidth="1"/>
+    <col min="4099" max="4099" width="76.6640625" customWidth="1"/>
+    <col min="4353" max="4353" width="19" customWidth="1"/>
+    <col min="4354" max="4354" width="79" customWidth="1"/>
+    <col min="4355" max="4355" width="76.6640625" customWidth="1"/>
+    <col min="4609" max="4609" width="19" customWidth="1"/>
+    <col min="4610" max="4610" width="79" customWidth="1"/>
+    <col min="4611" max="4611" width="76.6640625" customWidth="1"/>
+    <col min="4865" max="4865" width="19" customWidth="1"/>
+    <col min="4866" max="4866" width="79" customWidth="1"/>
+    <col min="4867" max="4867" width="76.6640625" customWidth="1"/>
+    <col min="5121" max="5121" width="19" customWidth="1"/>
+    <col min="5122" max="5122" width="79" customWidth="1"/>
+    <col min="5123" max="5123" width="76.6640625" customWidth="1"/>
+    <col min="5377" max="5377" width="19" customWidth="1"/>
+    <col min="5378" max="5378" width="79" customWidth="1"/>
+    <col min="5379" max="5379" width="76.6640625" customWidth="1"/>
+    <col min="5633" max="5633" width="19" customWidth="1"/>
+    <col min="5634" max="5634" width="79" customWidth="1"/>
+    <col min="5635" max="5635" width="76.6640625" customWidth="1"/>
+    <col min="5889" max="5889" width="19" customWidth="1"/>
+    <col min="5890" max="5890" width="79" customWidth="1"/>
+    <col min="5891" max="5891" width="76.6640625" customWidth="1"/>
+    <col min="6145" max="6145" width="19" customWidth="1"/>
+    <col min="6146" max="6146" width="79" customWidth="1"/>
+    <col min="6147" max="6147" width="76.6640625" customWidth="1"/>
+    <col min="6401" max="6401" width="19" customWidth="1"/>
+    <col min="6402" max="6402" width="79" customWidth="1"/>
+    <col min="6403" max="6403" width="76.6640625" customWidth="1"/>
+    <col min="6657" max="6657" width="19" customWidth="1"/>
+    <col min="6658" max="6658" width="79" customWidth="1"/>
+    <col min="6659" max="6659" width="76.6640625" customWidth="1"/>
+    <col min="6913" max="6913" width="19" customWidth="1"/>
+    <col min="6914" max="6914" width="79" customWidth="1"/>
+    <col min="6915" max="6915" width="76.6640625" customWidth="1"/>
+    <col min="7169" max="7169" width="19" customWidth="1"/>
+    <col min="7170" max="7170" width="79" customWidth="1"/>
+    <col min="7171" max="7171" width="76.6640625" customWidth="1"/>
+    <col min="7425" max="7425" width="19" customWidth="1"/>
+    <col min="7426" max="7426" width="79" customWidth="1"/>
+    <col min="7427" max="7427" width="76.6640625" customWidth="1"/>
+    <col min="7681" max="7681" width="19" customWidth="1"/>
+    <col min="7682" max="7682" width="79" customWidth="1"/>
+    <col min="7683" max="7683" width="76.6640625" customWidth="1"/>
+    <col min="7937" max="7937" width="19" customWidth="1"/>
+    <col min="7938" max="7938" width="79" customWidth="1"/>
+    <col min="7939" max="7939" width="76.6640625" customWidth="1"/>
+    <col min="8193" max="8193" width="19" customWidth="1"/>
+    <col min="8194" max="8194" width="79" customWidth="1"/>
+    <col min="8195" max="8195" width="76.6640625" customWidth="1"/>
+    <col min="8449" max="8449" width="19" customWidth="1"/>
+    <col min="8450" max="8450" width="79" customWidth="1"/>
+    <col min="8451" max="8451" width="76.6640625" customWidth="1"/>
+    <col min="8705" max="8705" width="19" customWidth="1"/>
+    <col min="8706" max="8706" width="79" customWidth="1"/>
+    <col min="8707" max="8707" width="76.6640625" customWidth="1"/>
+    <col min="8961" max="8961" width="19" customWidth="1"/>
+    <col min="8962" max="8962" width="79" customWidth="1"/>
+    <col min="8963" max="8963" width="76.6640625" customWidth="1"/>
+    <col min="9217" max="9217" width="19" customWidth="1"/>
+    <col min="9218" max="9218" width="79" customWidth="1"/>
+    <col min="9219" max="9219" width="76.6640625" customWidth="1"/>
+    <col min="9473" max="9473" width="19" customWidth="1"/>
+    <col min="9474" max="9474" width="79" customWidth="1"/>
+    <col min="9475" max="9475" width="76.6640625" customWidth="1"/>
+    <col min="9729" max="9729" width="19" customWidth="1"/>
+    <col min="9730" max="9730" width="79" customWidth="1"/>
+    <col min="9731" max="9731" width="76.6640625" customWidth="1"/>
+    <col min="9985" max="9985" width="19" customWidth="1"/>
+    <col min="9986" max="9986" width="79" customWidth="1"/>
+    <col min="9987" max="9987" width="76.6640625" customWidth="1"/>
+    <col min="10241" max="10241" width="19" customWidth="1"/>
+    <col min="10242" max="10242" width="79" customWidth="1"/>
+    <col min="10243" max="10243" width="76.6640625" customWidth="1"/>
+    <col min="10497" max="10497" width="19" customWidth="1"/>
+    <col min="10498" max="10498" width="79" customWidth="1"/>
+    <col min="10499" max="10499" width="76.6640625" customWidth="1"/>
+    <col min="10753" max="10753" width="19" customWidth="1"/>
+    <col min="10754" max="10754" width="79" customWidth="1"/>
+    <col min="10755" max="10755" width="76.6640625" customWidth="1"/>
+    <col min="11009" max="11009" width="19" customWidth="1"/>
+    <col min="11010" max="11010" width="79" customWidth="1"/>
+    <col min="11011" max="11011" width="76.6640625" customWidth="1"/>
+    <col min="11265" max="11265" width="19" customWidth="1"/>
+    <col min="11266" max="11266" width="79" customWidth="1"/>
+    <col min="11267" max="11267" width="76.6640625" customWidth="1"/>
+    <col min="11521" max="11521" width="19" customWidth="1"/>
+    <col min="11522" max="11522" width="79" customWidth="1"/>
+    <col min="11523" max="11523" width="76.6640625" customWidth="1"/>
+    <col min="11777" max="11777" width="19" customWidth="1"/>
+    <col min="11778" max="11778" width="79" customWidth="1"/>
+    <col min="11779" max="11779" width="76.6640625" customWidth="1"/>
+    <col min="12033" max="12033" width="19" customWidth="1"/>
+    <col min="12034" max="12034" width="79" customWidth="1"/>
+    <col min="12035" max="12035" width="76.6640625" customWidth="1"/>
+    <col min="12289" max="12289" width="19" customWidth="1"/>
+    <col min="12290" max="12290" width="79" customWidth="1"/>
+    <col min="12291" max="12291" width="76.6640625" customWidth="1"/>
+    <col min="12545" max="12545" width="19" customWidth="1"/>
+    <col min="12546" max="12546" width="79" customWidth="1"/>
+    <col min="12547" max="12547" width="76.6640625" customWidth="1"/>
+    <col min="12801" max="12801" width="19" customWidth="1"/>
+    <col min="12802" max="12802" width="79" customWidth="1"/>
+    <col min="12803" max="12803" width="76.6640625" customWidth="1"/>
+    <col min="13057" max="13057" width="19" customWidth="1"/>
+    <col min="13058" max="13058" width="79" customWidth="1"/>
+    <col min="13059" max="13059" width="76.6640625" customWidth="1"/>
+    <col min="13313" max="13313" width="19" customWidth="1"/>
+    <col min="13314" max="13314" width="79" customWidth="1"/>
+    <col min="13315" max="13315" width="76.6640625" customWidth="1"/>
+    <col min="13569" max="13569" width="19" customWidth="1"/>
+    <col min="13570" max="13570" width="79" customWidth="1"/>
+    <col min="13571" max="13571" width="76.6640625" customWidth="1"/>
+    <col min="13825" max="13825" width="19" customWidth="1"/>
+    <col min="13826" max="13826" width="79" customWidth="1"/>
+    <col min="13827" max="13827" width="76.6640625" customWidth="1"/>
+    <col min="14081" max="14081" width="19" customWidth="1"/>
+    <col min="14082" max="14082" width="79" customWidth="1"/>
+    <col min="14083" max="14083" width="76.6640625" customWidth="1"/>
+    <col min="14337" max="14337" width="19" customWidth="1"/>
+    <col min="14338" max="14338" width="79" customWidth="1"/>
+    <col min="14339" max="14339" width="76.6640625" customWidth="1"/>
+    <col min="14593" max="14593" width="19" customWidth="1"/>
+    <col min="14594" max="14594" width="79" customWidth="1"/>
+    <col min="14595" max="14595" width="76.6640625" customWidth="1"/>
+    <col min="14849" max="14849" width="19" customWidth="1"/>
+    <col min="14850" max="14850" width="79" customWidth="1"/>
+    <col min="14851" max="14851" width="76.6640625" customWidth="1"/>
+    <col min="15105" max="15105" width="19" customWidth="1"/>
+    <col min="15106" max="15106" width="79" customWidth="1"/>
+    <col min="15107" max="15107" width="76.6640625" customWidth="1"/>
+    <col min="15361" max="15361" width="19" customWidth="1"/>
+    <col min="15362" max="15362" width="79" customWidth="1"/>
+    <col min="15363" max="15363" width="76.6640625" customWidth="1"/>
+    <col min="15617" max="15617" width="19" customWidth="1"/>
+    <col min="15618" max="15618" width="79" customWidth="1"/>
+    <col min="15619" max="15619" width="76.6640625" customWidth="1"/>
+    <col min="15873" max="15873" width="19" customWidth="1"/>
+    <col min="15874" max="15874" width="79" customWidth="1"/>
+    <col min="15875" max="15875" width="76.6640625" customWidth="1"/>
+    <col min="16129" max="16129" width="19" customWidth="1"/>
+    <col min="16130" max="16130" width="79" customWidth="1"/>
+    <col min="16131" max="16131" width="76.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="32.049999999999997" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:3" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="18">
         <v>9999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="78" x14ac:dyDescent="0.6">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1345,72 +1289,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.27734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.94140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.0546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.27734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.609375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.94140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.27734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>36</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1422,231 +1366,237 @@
       <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
+      <c r="R1" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>77</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="9"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A4" s="8" t="s">
+      <c r="Q3" s="7"/>
+      <c r="R3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>79</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A5" s="8" t="s">
+      <c r="Q4" s="7"/>
+      <c r="R4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K5" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="9"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A7" s="8" t="s">
+      <c r="Q6" s="7"/>
+      <c r="R6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>81</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>